<commit_message>
File Refactoring and Defaults Editing
This commit removes some template files.

- Content file refactoring.
- Added Ravine map.
- Two Ravine submaps are included in this commit but are not used. They
will be removed in the next commit.
- Added FValorHeroInitializationProperties struct to store some
initialization properties, similar to ValorCharacterStatContainer. These
exist to make replication of stats easier and reduces the number of
network requests for replication.
- Added UValorUserWidget parent class for all future UUserWidgets to
extend from. The intent is to reduce editor autocomplete cluttering and
allow some code implementation of potentially critical sections.
- Added EValorTeam::Invalid as a hidden enum value. Even though UENUM
with flags will assign the first value 1, the same can not be said of
native usage. None will be assigned a value of 0U which can't be used in
flag operations.
</commit_message>
<xml_diff>
--- a/Content/Data/Stats/HeroStats.xlsx
+++ b/Content/Data/Stats/HeroStats.xlsx
@@ -14,6 +14,13 @@
   <sheets>
     <sheet name="Default" sheetId="2" r:id="rId1"/>
     <sheet name="Natsu" sheetId="1" r:id="rId2"/>
+    <sheet name="Finn" sheetId="3" r:id="rId3"/>
+    <sheet name="Shaari" sheetId="4" r:id="rId4"/>
+    <sheet name="Bhaskara" sheetId="5" r:id="rId5"/>
+    <sheet name="Reva" sheetId="6" r:id="rId6"/>
+    <sheet name="Shan'dal" sheetId="7" r:id="rId7"/>
+    <sheet name="Jaylin" sheetId="8" r:id="rId8"/>
+    <sheet name="Scrow" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1841,4 +1848,88 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>